<commit_message>
Updated Planning XLSX Sheet (Arny Commit #16)
</commit_message>
<xml_diff>
--- a/SubRoutine Diagrams/Planning.xlsx
+++ b/SubRoutine Diagrams/Planning.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\TimeSheet\InsemiTimeSheet\SubRoutine Diagrams\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\TimeSheet\_OFFICIAL_\InsemiTimeSheet\SubRoutine Diagrams\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B9775FD-5775-4634-AF74-7178FD4DD9E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50726C37-C74F-4242-A8A9-BD0E45753A90}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{10764AD2-775D-4E13-9BB5-0EEC0859F0D7}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="67">
   <si>
     <t>Website Infrastructure Set-Up</t>
   </si>
@@ -222,6 +222,18 @@
   </si>
   <si>
     <t>React learning + Basic DB Setup</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SQL </t>
+  </si>
+  <si>
+    <t>Daily Activity - Per User</t>
+  </si>
+  <si>
+    <t>All User Data - Secure</t>
+  </si>
+  <si>
+    <t>Leave Data - Per User</t>
   </si>
 </sst>
 </file>
@@ -582,8 +594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71435A39-65CF-484A-8CA3-509D1C8BD591}">
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -816,39 +828,51 @@
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>42</v>
       </c>
       <c r="B17" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="D17" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>44</v>
       </c>
       <c r="B18" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="D18" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>45</v>
       </c>
       <c r="B19" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="D19" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>46</v>
       </c>
       <c r="B20" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="D20" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>47</v>
       </c>
@@ -856,7 +880,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>49</v>
       </c>
@@ -864,12 +888,12 @@
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>55</v>
       </c>
@@ -877,7 +901,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>42</v>
       </c>
@@ -885,7 +909,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>44</v>
       </c>
@@ -893,7 +917,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>45</v>
       </c>
@@ -901,7 +925,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>46</v>
       </c>
@@ -909,7 +933,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>47</v>
       </c>
@@ -917,7 +941,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>61</v>
       </c>

</xml_diff>

<commit_message>
Integrated Calendar with Project (Arny Commit #18)
</commit_message>
<xml_diff>
--- a/SubRoutine Diagrams/Planning.xlsx
+++ b/SubRoutine Diagrams/Planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\TimeSheet\_OFFICIAL_\InsemiTimeSheet\SubRoutine Diagrams\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50726C37-C74F-4242-A8A9-BD0E45753A90}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71CCBCE0-FB15-45B2-BAEA-2286E2370E5C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{10764AD2-775D-4E13-9BB5-0EEC0859F0D7}"/>
   </bookViews>
@@ -595,7 +595,7 @@
   <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Updated Planning (Arny Commit #21)
</commit_message>
<xml_diff>
--- a/SubRoutine Diagrams/Planning.xlsx
+++ b/SubRoutine Diagrams/Planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\TimeSheet\_OFFICIAL_\InsemiTimeSheet\SubRoutine Diagrams\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71CCBCE0-FB15-45B2-BAEA-2286E2370E5C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C588E358-49B4-4EB2-AA8D-249899FDA15E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{10764AD2-775D-4E13-9BB5-0EEC0859F0D7}"/>
   </bookViews>
@@ -249,7 +249,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -262,8 +262,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -271,13 +283,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -594,8 +623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71435A39-65CF-484A-8CA3-509D1C8BD591}">
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -614,16 +643,16 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="A2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="E2" s="1" t="s">
@@ -637,16 +666,16 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="A3" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="E3" s="1" t="s">
@@ -660,16 +689,16 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="A4" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E4" s="1" t="s">
@@ -683,16 +712,16 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="A5" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E5" s="1" t="s">
@@ -706,16 +735,16 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="A6" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E6" s="1" t="s">
@@ -723,16 +752,16 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="A7" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
@@ -740,16 +769,16 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+      <c r="A8" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E8" s="1" t="s">
@@ -757,16 +786,16 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+      <c r="A9" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E9" s="1" t="s">
@@ -774,16 +803,16 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+      <c r="A10" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E10" s="1" t="s">
@@ -791,10 +820,10 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="C11" t="s">
+      <c r="C11" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E11" s="1" t="s">
@@ -802,10 +831,10 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="C12" t="s">
+      <c r="C12" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E12" s="1" t="s">
@@ -813,10 +842,10 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="C13" t="s">
+      <c r="C13" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E13" s="1" t="s">

</xml_diff>

<commit_message>
Planning for Week 6
</commit_message>
<xml_diff>
--- a/SubRoutine Diagrams/Planning.xlsx
+++ b/SubRoutine Diagrams/Planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\TimeSheet\_OFFICIAL_\InsemiTimeSheet\SubRoutine Diagrams\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EB1BC49-FE6E-4CE5-9960-B73D773E2CD0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66AE405B-9998-487B-83F0-740EB06905D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{10764AD2-775D-4E13-9BB5-0EEC0859F0D7}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="101">
   <si>
     <t>Website Infrastructure Set-Up</t>
   </si>
@@ -300,6 +300,42 @@
   </si>
   <si>
     <t xml:space="preserve">Client Customization </t>
+  </si>
+  <si>
+    <t>Week 6</t>
+  </si>
+  <si>
+    <t>The options</t>
+  </si>
+  <si>
+    <t>User info</t>
+  </si>
+  <si>
+    <t>Manage permissions within the current user model</t>
+  </si>
+  <si>
+    <t>Integrate permissions into existing</t>
+  </si>
+  <si>
+    <t>Integrate User Model with Existing Apps</t>
+  </si>
+  <si>
+    <t>TimeTracker</t>
+  </si>
+  <si>
+    <t>HomeScreen</t>
+  </si>
+  <si>
+    <t>Arnav, Lohit</t>
+  </si>
+  <si>
+    <t>Shivam and Sid</t>
+  </si>
+  <si>
+    <t>Arnav and Shivam</t>
+  </si>
+  <si>
+    <t>Loh-dant</t>
   </si>
 </sst>
 </file>
@@ -702,16 +738,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71435A39-65CF-484A-8CA3-509D1C8BD591}">
-  <dimension ref="A1:H46"/>
+  <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="D58" sqref="D58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="29.90625" customWidth="1"/>
-    <col min="2" max="2" width="55" customWidth="1"/>
+    <col min="2" max="2" width="39.453125" customWidth="1"/>
     <col min="3" max="4" width="30.54296875" customWidth="1"/>
     <col min="5" max="5" width="31.08984375" customWidth="1"/>
     <col min="7" max="7" width="31.453125" customWidth="1"/>
@@ -1209,6 +1245,60 @@
         <v>80</v>
       </c>
     </row>
+    <row r="49" spans="1:4">
+      <c r="A49" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" t="s">
+        <v>94</v>
+      </c>
+      <c r="B50" t="s">
+        <v>95</v>
+      </c>
+      <c r="C50" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="B51" t="s">
+        <v>2</v>
+      </c>
+      <c r="C51" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" t="s">
+        <v>96</v>
+      </c>
+      <c r="B52" t="s">
+        <v>90</v>
+      </c>
+      <c r="C52" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" t="s">
+        <v>99</v>
+      </c>
+      <c r="B53" t="s">
+        <v>91</v>
+      </c>
+      <c r="C53" t="s">
+        <v>93</v>
+      </c>
+      <c r="D53" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="B54" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
User Imported Into React
</commit_message>
<xml_diff>
--- a/SubRoutine Diagrams/Planning.xlsx
+++ b/SubRoutine Diagrams/Planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\TimeSheet\_OFFICIAL_\InsemiTimeSheet\SubRoutine Diagrams\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66AE405B-9998-487B-83F0-740EB06905D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{781FE997-6523-45FD-9E4E-0B24940E9ED4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{10764AD2-775D-4E13-9BB5-0EEC0859F0D7}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="100">
   <si>
     <t>Website Infrastructure Set-Up</t>
   </si>
@@ -333,16 +333,13 @@
   </si>
   <si>
     <t>Arnav and Shivam</t>
-  </si>
-  <si>
-    <t>Loh-dant</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -357,6 +354,19 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFC000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -415,7 +425,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -424,6 +434,8 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -738,10 +750,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71435A39-65CF-484A-8CA3-509D1C8BD591}">
-  <dimension ref="A1:H54"/>
+  <dimension ref="A1:H58"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="D58" sqref="D58"/>
+      <selection activeCell="A52" sqref="A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1245,12 +1257,12 @@
         <v>80</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:3">
       <c r="A49" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:3">
       <c r="A50" t="s">
         <v>94</v>
       </c>
@@ -1261,7 +1273,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:3">
       <c r="B51" t="s">
         <v>2</v>
       </c>
@@ -1269,34 +1281,35 @@
         <v>98</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
-      <c r="A52" t="s">
+    <row r="52" spans="1:3">
+      <c r="A52" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B52" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="C52" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4">
+    </row>
+    <row r="53" spans="1:3">
       <c r="A53" t="s">
         <v>99</v>
       </c>
       <c r="B53" t="s">
         <v>91</v>
       </c>
-      <c r="C53" t="s">
+    </row>
+    <row r="54" spans="1:3">
+      <c r="B54" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" t="s">
         <v>93</v>
-      </c>
-      <c r="D53" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4">
-      <c r="B54" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Planning Updated (Arny Commit #46)
</commit_message>
<xml_diff>
--- a/SubRoutine Diagrams/Planning.xlsx
+++ b/SubRoutine Diagrams/Planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\TimeSheet\_OFFICIAL_\InsemiTimeSheet\SubRoutine Diagrams\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{781FE997-6523-45FD-9E4E-0B24940E9ED4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBB94219-8B44-4116-8239-3059FE098F26}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{10764AD2-775D-4E13-9BB5-0EEC0859F0D7}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="107">
   <si>
     <t>Website Infrastructure Set-Up</t>
   </si>
@@ -333,6 +333,27 @@
   </si>
   <si>
     <t>Arnav and Shivam</t>
+  </si>
+  <si>
+    <t>Week 7</t>
+  </si>
+  <si>
+    <t>Settings Panel</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Hierarchy With Existing User Levels</t>
+  </si>
+  <si>
+    <t>Sid + Shivam</t>
+  </si>
+  <si>
+    <t>Lohit + Arnav</t>
+  </si>
+  <si>
+    <t>Arny + Shivam</t>
+  </si>
+  <si>
+    <t>Lohit (due to refusal to contact Sid)</t>
   </si>
 </sst>
 </file>
@@ -372,7 +393,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -394,6 +415,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -425,7 +458,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -436,6 +469,12 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -750,10 +789,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71435A39-65CF-484A-8CA3-509D1C8BD591}">
-  <dimension ref="A1:H58"/>
+  <dimension ref="A1:H62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1302,17 +1341,62 @@
         <v>10</v>
       </c>
     </row>
+    <row r="56" spans="1:3">
+      <c r="A56" t="s">
+        <v>100</v>
+      </c>
+    </row>
     <row r="57" spans="1:3">
-      <c r="A57" t="s">
+      <c r="A57" s="9" t="s">
         <v>92</v>
       </c>
+      <c r="C57" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="58" spans="1:3">
-      <c r="A58" t="s">
+      <c r="A58" s="9" t="s">
         <v>93</v>
       </c>
     </row>
+    <row r="59" spans="1:3">
+      <c r="A59" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="B59" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C59" s="11" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" s="8"/>
+      <c r="B60" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C60" s="11"/>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="C61" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="C62" t="s">
+        <v>104</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C59:C60"/>
+  </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Export GUI Created (Arny Commit #46)
</commit_message>
<xml_diff>
--- a/SubRoutine Diagrams/Planning.xlsx
+++ b/SubRoutine Diagrams/Planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\TimeSheet\_OFFICIAL_\InsemiTimeSheet\SubRoutine Diagrams\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBB94219-8B44-4116-8239-3059FE098F26}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DDFA2C5-4AD5-47A9-8A61-6CE8D1B62712}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{10764AD2-775D-4E13-9BB5-0EEC0859F0D7}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="117">
   <si>
     <t>Website Infrastructure Set-Up</t>
   </si>
@@ -314,9 +314,6 @@
     <t>Manage permissions within the current user model</t>
   </si>
   <si>
-    <t>Integrate permissions into existing</t>
-  </si>
-  <si>
     <t>Integrate User Model with Existing Apps</t>
   </si>
   <si>
@@ -353,7 +350,40 @@
     <t>Arny + Shivam</t>
   </si>
   <si>
-    <t>Lohit (due to refusal to contact Sid)</t>
+    <t>Week 8</t>
+  </si>
+  <si>
+    <t>Fetch Choices API</t>
+  </si>
+  <si>
+    <t>Create Assignments</t>
+  </si>
+  <si>
+    <t>Integration with User</t>
+  </si>
+  <si>
+    <t>Leave System Card</t>
+  </si>
+  <si>
+    <t>Lohit &amp; Sid</t>
+  </si>
+  <si>
+    <t>User Model</t>
+  </si>
+  <si>
+    <t>Permissions</t>
+  </si>
+  <si>
+    <t>Inter-UserType</t>
+  </si>
+  <si>
+    <t>Intra-UserType</t>
+  </si>
+  <si>
+    <t>Research and Implementation</t>
+  </si>
+  <si>
+    <t>Inter-user relationship</t>
   </si>
 </sst>
 </file>
@@ -789,10 +819,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71435A39-65CF-484A-8CA3-509D1C8BD591}">
-  <dimension ref="A1:H62"/>
+  <dimension ref="A1:H75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="C64" sqref="C64"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="A70" sqref="A70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -924,7 +954,7 @@
         <v>33</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>7</v>
+        <v>111</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>23</v>
@@ -941,7 +971,7 @@
         <v>34</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>7</v>
+        <v>112</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>21</v>
@@ -1303,13 +1333,13 @@
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
+        <v>93</v>
+      </c>
+      <c r="B50" t="s">
         <v>94</v>
       </c>
-      <c r="B50" t="s">
-        <v>95</v>
-      </c>
       <c r="C50" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -1317,12 +1347,12 @@
         <v>2</v>
       </c>
       <c r="C51" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B52" s="7" t="s">
         <v>90</v>
@@ -1330,7 +1360,7 @@
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B53" t="s">
         <v>91</v>
@@ -1343,59 +1373,100 @@
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="C57" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="B58" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C58" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" s="8"/>
+      <c r="B59" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C59" s="11"/>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" s="10" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="57" spans="1:3">
-      <c r="A57" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="C57" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3">
-      <c r="A58" s="9" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3">
-      <c r="A59" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="B59" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C59" s="11" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3">
-      <c r="A60" s="8"/>
-      <c r="B60" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="C60" s="11"/>
+      <c r="C60" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="61" spans="1:3">
-      <c r="A61" s="10" t="s">
+      <c r="A61" s="9" t="s">
         <v>101</v>
       </c>
       <c r="C61" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="62" spans="1:3">
-      <c r="A62" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="C62" t="s">
-        <v>104</v>
+    <row r="63" spans="1:3">
+      <c r="A63" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64" t="s">
+        <v>115</v>
+      </c>
+      <c r="B64" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="B65" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="B66" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="A72" t="s">
+        <v>10</v>
+      </c>
+      <c r="B72" s="9" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="B73" s="9" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="B74" s="9" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="A75" s="9" t="s">
+        <v>107</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="C59:C60"/>
+    <mergeCell ref="C58:C59"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Login Authentication Problems Fixed (Team Commit #1)
</commit_message>
<xml_diff>
--- a/SubRoutine Diagrams/Planning.xlsx
+++ b/SubRoutine Diagrams/Planning.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\TimeSheet\_OFFICIAL_\InsemiTimeSheet\SubRoutine Diagrams\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DDFA2C5-4AD5-47A9-8A61-6CE8D1B62712}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5680535A-4B1A-4523-9A02-1623812229DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{10764AD2-775D-4E13-9BB5-0EEC0859F0D7}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{10764AD2-775D-4E13-9BB5-0EEC0859F0D7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="116">
   <si>
     <t>Website Infrastructure Set-Up</t>
   </si>
@@ -140,9 +140,6 @@
     <t>Week 7 (29.06.2020 - 5.07.2020)</t>
   </si>
   <si>
-    <t>Week 8 (5.07.2020 - 11.07.2020)</t>
-  </si>
-  <si>
     <t>Week 2</t>
   </si>
   <si>
@@ -281,15 +278,6 @@
     <t xml:space="preserve">1. SEARCH BAR </t>
   </si>
   <si>
-    <t>Week 9 (11.07.2020 - 17.07.2020)</t>
-  </si>
-  <si>
-    <t>Week 10 (18.07.2020-24.07.2020)</t>
-  </si>
-  <si>
-    <t>Week 11 (25.07.2020 - 31.07.2020)</t>
-  </si>
-  <si>
     <t>Week 12 (01.08.2020 - 07.08.20)</t>
   </si>
   <si>
@@ -299,9 +287,6 @@
     <t xml:space="preserve"> Time Sheet Viewer</t>
   </si>
   <si>
-    <t xml:space="preserve">Client Customization </t>
-  </si>
-  <si>
     <t>Week 6</t>
   </si>
   <si>
@@ -384,6 +369,18 @@
   </si>
   <si>
     <t>Inter-user relationship</t>
+  </si>
+  <si>
+    <t>Week 8 (6.07.2020 - 12.07.2020)</t>
+  </si>
+  <si>
+    <t>Week 9 (03.08.2020 - 09.08.2020)</t>
+  </si>
+  <si>
+    <t>Week 10 (10.08.2020-16.08.2020)</t>
+  </si>
+  <si>
+    <t>Week 11 (17.08.2020 - 23.08.2020)</t>
   </si>
 </sst>
 </file>
@@ -821,8 +818,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71435A39-65CF-484A-8CA3-509D1C8BD591}">
   <dimension ref="A1:H75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="A70" sqref="A70"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -937,7 +934,7 @@
         <v>31</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>23</v>
@@ -954,7 +951,7 @@
         <v>33</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>23</v>
@@ -971,7 +968,7 @@
         <v>34</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>21</v>
@@ -985,11 +982,9 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>10</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="B9" s="3"/>
       <c r="C9" s="2" t="s">
         <v>23</v>
       </c>
@@ -1002,10 +997,10 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="3" t="s">
-        <v>82</v>
+        <v>113</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>1</v>
+        <v>107</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>22</v>
@@ -1019,10 +1014,10 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="3" t="s">
-        <v>83</v>
+        <v>114</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>88</v>
+        <v>1</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>21</v>
@@ -1036,7 +1031,7 @@
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="3" t="s">
-        <v>84</v>
+        <v>115</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>6</v>
@@ -1053,7 +1048,7 @@
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="3" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>11</v>
@@ -1070,7 +1065,7 @@
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="3" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>4</v>
@@ -1082,125 +1077,125 @@
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" t="s">
         <v>37</v>
       </c>
-      <c r="B17" t="s">
-        <v>38</v>
-      </c>
       <c r="D17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21" t="s">
         <v>42</v>
-      </c>
-      <c r="B21" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B25" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B26" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B27" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B28" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B29" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B30" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B31" t="s">
         <v>24</v>
@@ -1208,138 +1203,138 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C33" s="4"/>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B34" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C34" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D34" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B35" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C35" t="s">
         <v>21</v>
       </c>
       <c r="D35" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B36" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C36" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D36" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B37" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C37" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D37" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B38" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B39" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B40" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
+        <v>74</v>
+      </c>
+      <c r="B43" t="s">
         <v>75</v>
-      </c>
-      <c r="B43" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="B44" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B45" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" t="s">
+        <v>78</v>
+      </c>
+      <c r="B46" t="s">
         <v>79</v>
-      </c>
-      <c r="B46" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B50" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C50" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -1347,23 +1342,23 @@
         <v>2</v>
       </c>
       <c r="C51" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" s="6" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B53" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="54" spans="1:3">
@@ -1373,26 +1368,26 @@
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" s="10" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C57" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58" s="8" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B58" s="8" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C58" s="11" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="59" spans="1:3">
@@ -1404,41 +1399,41 @@
     </row>
     <row r="60" spans="1:3">
       <c r="A60" s="10" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C60" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61" s="9" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C61" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="63" spans="1:3">
       <c r="A63" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B64" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="B65" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="B66" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -1446,22 +1441,22 @@
         <v>10</v>
       </c>
       <c r="B72" s="9" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="B73" s="9" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="74" spans="1:2">
       <c r="B74" s="9" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
     </row>
     <row r="75" spans="1:2">
       <c r="A75" s="9" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Basic Prototype Ready! (Team Commit #2)
</commit_message>
<xml_diff>
--- a/SubRoutine Diagrams/Planning.xlsx
+++ b/SubRoutine Diagrams/Planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\TimeSheet\_OFFICIAL_\InsemiTimeSheet\SubRoutine Diagrams\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5680535A-4B1A-4523-9A02-1623812229DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A86FAA81-D2FE-47E2-8E64-AE313C639155}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{10764AD2-775D-4E13-9BB5-0EEC0859F0D7}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="131">
   <si>
     <t>Website Infrastructure Set-Up</t>
   </si>
@@ -381,6 +381,51 @@
   </si>
   <si>
     <t>Week 11 (17.08.2020 - 23.08.2020)</t>
+  </si>
+  <si>
+    <t>TimeSheet UI</t>
+  </si>
+  <si>
+    <t>Data Export</t>
+  </si>
+  <si>
+    <t>Wed</t>
+  </si>
+  <si>
+    <t>Thu</t>
+  </si>
+  <si>
+    <t>Fri</t>
+  </si>
+  <si>
+    <t>Sat</t>
+  </si>
+  <si>
+    <t>Sid</t>
+  </si>
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>Basic Setup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Frontend </t>
+  </si>
+  <si>
+    <t>Django</t>
+  </si>
+  <si>
+    <t>Frontend</t>
+  </si>
+  <si>
+    <t>Data Collection</t>
+  </si>
+  <si>
+    <t>Updation in Activity Report</t>
+  </si>
+  <si>
+    <t>Choices API Integration</t>
   </si>
 </sst>
 </file>
@@ -816,10 +861,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71435A39-65CF-484A-8CA3-509D1C8BD591}">
-  <dimension ref="A1:H75"/>
+  <dimension ref="A1:H83"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="A85" sqref="A85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1000,7 +1045,7 @@
         <v>113</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>22</v>
@@ -1017,7 +1062,7 @@
         <v>114</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>1</v>
+        <v>107</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>21</v>
@@ -1034,7 +1079,7 @@
         <v>115</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>6</v>
+        <v>117</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>21</v>
@@ -1426,17 +1471,17 @@
         <v>108</v>
       </c>
     </row>
-    <row r="65" spans="1:2">
+    <row r="65" spans="1:5">
       <c r="B65" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="66" spans="1:2">
+    <row r="66" spans="1:5">
       <c r="B66" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="72" spans="1:2">
+    <row r="72" spans="1:5">
       <c r="A72" t="s">
         <v>10</v>
       </c>
@@ -1444,19 +1489,101 @@
         <v>101</v>
       </c>
     </row>
-    <row r="73" spans="1:2">
+    <row r="73" spans="1:5">
       <c r="B73" s="9" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="74" spans="1:2">
+    <row r="74" spans="1:5">
       <c r="B74" s="9" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="75" spans="1:2">
+    <row r="75" spans="1:5">
       <c r="A75" s="9" t="s">
         <v>102</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
+      <c r="B79" t="s">
+        <v>123</v>
+      </c>
+      <c r="C79" t="s">
+        <v>13</v>
+      </c>
+      <c r="D79" t="s">
+        <v>122</v>
+      </c>
+      <c r="E79" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5">
+      <c r="A80" t="s">
+        <v>118</v>
+      </c>
+      <c r="B80" t="s">
+        <v>124</v>
+      </c>
+      <c r="C80" t="s">
+        <v>125</v>
+      </c>
+      <c r="D80" t="s">
+        <v>126</v>
+      </c>
+      <c r="E80" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
+      <c r="A81" t="s">
+        <v>119</v>
+      </c>
+      <c r="B81" t="s">
+        <v>124</v>
+      </c>
+      <c r="C81" t="s">
+        <v>125</v>
+      </c>
+      <c r="D81" t="s">
+        <v>126</v>
+      </c>
+      <c r="E81" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5">
+      <c r="A82" t="s">
+        <v>120</v>
+      </c>
+      <c r="B82" t="s">
+        <v>127</v>
+      </c>
+      <c r="C82" t="s">
+        <v>128</v>
+      </c>
+      <c r="D82" t="s">
+        <v>129</v>
+      </c>
+      <c r="E82" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5">
+      <c r="A83" t="s">
+        <v>121</v>
+      </c>
+      <c r="B83" t="s">
+        <v>127</v>
+      </c>
+      <c r="C83" t="s">
+        <v>128</v>
+      </c>
+      <c r="D83" t="s">
+        <v>129</v>
+      </c>
+      <c r="E83" t="s">
+        <v>130</v>
       </c>
     </row>
   </sheetData>

</xml_diff>